<commit_message>
add transmittal function edited
export to excel function
- saved to C:\Users\Public\tracer_exports
</commit_message>
<xml_diff>
--- a/public/assets/format.xlsx
+++ b/public/assets/format.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jane Martinez Pili\OneDrive\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jane Martinez Pili\PhilPostSys\public\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C52E3EB3-4696-49B0-BD4E-2456A522AEDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEB55E14-B8AA-47AA-85B3-F6EB17C7E5D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{4880FD3E-A64B-47FA-99F1-F196802745F4}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>PHILIPPINE POSTAL CORPORATION</t>
   </si>
@@ -52,12 +52,6 @@
   </si>
   <si>
     <t>Sir / Madam:</t>
-  </si>
-  <si>
-    <t>DepEd Albay, Bogtong Road,</t>
-  </si>
-  <si>
-    <t>Legazpi City</t>
   </si>
   <si>
     <t>Transmitted are encoded Registry Return Recepits/Proofs of Delivery with the following Tracking Numbers, for your appropriate action please.</t>
@@ -137,7 +131,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -165,16 +159,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -547,7 +540,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:C8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -557,36 +550,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
     </row>
     <row r="2" spans="1:9" ht="15.75">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
     </row>
     <row r="3" spans="1:9" ht="15.75">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="14" t="s">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="1"/>
@@ -595,19 +585,19 @@
       <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:9" ht="15" customHeight="1">
-      <c r="A7" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
+      <c r="A7" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
       <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:9" ht="15" customHeight="1">
-      <c r="A8" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
+      <c r="A8" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
       <c r="D8" s="2"/>
     </row>
     <row r="9" spans="1:9" ht="15" customHeight="1">
@@ -617,17 +607,13 @@
       <c r="D9" s="2"/>
     </row>
     <row r="10" spans="1:9" ht="15" customHeight="1">
-      <c r="A10" s="8" t="s">
-        <v>5</v>
-      </c>
+      <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
       <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:9" ht="15.75">
-      <c r="A11" s="6" t="s">
-        <v>6</v>
-      </c>
+      <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="3"/>
@@ -646,7 +632,7 @@
     </row>
     <row r="15" spans="1:9" ht="15" customHeight="1">
       <c r="A15" s="8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>

</xml_diff>

<commit_message>
export to excel function updated
- modal
- included rrr_tn content
</commit_message>
<xml_diff>
--- a/public/assets/format.xlsx
+++ b/public/assets/format.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jane Martinez Pili\PhilPostSys\public\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEB55E14-B8AA-47AA-85B3-F6EB17C7E5D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6D38107-3E68-44BE-BAC5-7EA862CD2CA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{4880FD3E-A64B-47FA-99F1-F196802745F4}"/>
   </bookViews>
@@ -67,7 +67,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -99,11 +99,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF1C1E21"/>
-      <name val="Inherit"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FF1C1E21"/>
       <name val="Calibri"/>
@@ -131,7 +126,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -142,17 +137,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -166,6 +155,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -537,134 +529,329 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7DE82DE-791B-46DF-B022-77B4FAB2DFF7}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="4" width="20.7109375" customWidth="1"/>
     <col min="5" max="5" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-    </row>
-    <row r="2" spans="1:9" ht="15.75">
-      <c r="A2" s="11" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-    </row>
-    <row r="3" spans="1:9" ht="15.75">
-      <c r="A3" s="10" t="s">
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1">
-      <c r="A7" s="12" t="s">
+    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1">
-      <c r="A8" s="13" t="s">
+    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
+    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+    </row>
+    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:9" ht="15.75">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
+    <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:9" ht="15.75">
-      <c r="A13" s="9" t="s">
+    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="9"/>
-    </row>
-    <row r="15" spans="1:9" ht="15" customHeight="1">
-      <c r="A15" s="8" t="s">
+      <c r="B13" s="7"/>
+    </row>
+    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="4"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:9" ht="15" customHeight="1">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="6"/>
+    <row r="16" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="4"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
     </row>
-    <row r="18" spans="1:4" ht="15.75">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="4"/>
+    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="12"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+    </row>
+    <row r="25" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+    </row>
+    <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+    </row>
+    <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+    </row>
+    <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+    </row>
+    <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+    </row>
+    <row r="31" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+    </row>
+    <row r="32" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+    </row>
+    <row r="33" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="5"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+    </row>
+    <row r="34" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="5"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+    </row>
+    <row r="35" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="5"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+    </row>
+    <row r="36" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="5"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+    </row>
+    <row r="37" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="5"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+    </row>
+    <row r="38" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="5"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+    </row>
+    <row r="39" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="5"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+    </row>
+    <row r="40" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="5"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+    </row>
+    <row r="41" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="5"/>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+    </row>
+    <row r="42" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="5"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+    </row>
+    <row r="43" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="5"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+    </row>
+    <row r="44" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="5"/>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+    </row>
+    <row r="45" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="5"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+    </row>
+    <row r="46" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="5"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+    </row>
+    <row r="47" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="5"/>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+    </row>
+    <row r="48" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="5"/>
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
+    </row>
+    <row r="49" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="5"/>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+    </row>
+    <row r="50" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="5"/>
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+    </row>
+    <row r="51" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="5"/>
+      <c r="B51" s="5"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
     <mergeCell ref="A15:D16"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A10:C10"/>
@@ -673,6 +860,7 @@
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:D9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
2 page export function
</commit_message>
<xml_diff>
--- a/public/assets/format.xlsx
+++ b/public/assets/format.xlsx
@@ -8,16 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d15d29cc27c951d7/Documents/GitHub/PhilPostSys/PhilPostSys/public/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{D6D38107-3E68-44BE-BAC5-7EA862CD2CA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5DCBE765-6E6B-4B3D-92C4-D38E99EA0AAB}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{D6D38107-3E68-44BE-BAC5-7EA862CD2CA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1AD5F049-024D-4D26-A980-1F33D5AC36F4}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{4880FD3E-A64B-47FA-99F1-F196802745F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$D$42</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -531,8 +528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7DE82DE-791B-46DF-B022-77B4FAB2DFF7}">
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updated - blades and export format
</commit_message>
<xml_diff>
--- a/public/assets/format.xlsx
+++ b/public/assets/format.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d15d29cc27c951d7/Documents/GitHub/PhilPostSys/PhilPostSys/public/assets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jane Martinez Pili\OneDrive\Documents\GitHub\PhilPostSys\PhilPostSys\public\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{D6D38107-3E68-44BE-BAC5-7EA862CD2CA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1AD5F049-024D-4D26-A980-1F33D5AC36F4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC425D34-EF95-4FAF-83AA-A78DE2279417}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{4880FD3E-A64B-47FA-99F1-F196802745F4}"/>
   </bookViews>
@@ -51,13 +51,13 @@
     <t>Sir / Madam:</t>
   </si>
   <si>
-    <t>Transmitted are encoded Registry Return Recepits/Proofs of Delivery with the following Tracking Numbers, for your appropriate action please.</t>
-  </si>
-  <si>
     <t>REGIONAL OFFICE NO. 5</t>
   </si>
   <si>
     <t>DEPARTMENT OF EDUCATION</t>
+  </si>
+  <si>
+    <t>Transmitted are Registry Return Recepits/Proofs of Delivery with the following Tracking Numbers, for your appropriate action please.</t>
   </si>
 </sst>
 </file>
@@ -529,7 +529,7 @@
   <dimension ref="A1:I50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A14" sqref="A14:D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,7 +575,7 @@
     </row>
     <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
@@ -583,7 +583,7 @@
     </row>
     <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
@@ -615,7 +615,7 @@
     </row>
     <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>

</xml_diff>

<commit_message>
string manip - reports gen
</commit_message>
<xml_diff>
--- a/public/assets/format.xlsx
+++ b/public/assets/format.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jane Martinez Pili\OneDrive\Documents\GitHub\PhilPostSys\PhilPostSys\public\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC425D34-EF95-4FAF-83AA-A78DE2279417}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B7D8C2A-4300-4B6E-B85B-D36482ADAC3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{4880FD3E-A64B-47FA-99F1-F196802745F4}"/>
   </bookViews>
@@ -526,10 +526,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7DE82DE-791B-46DF-B022-77B4FAB2DFF7}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:D15"/>
+      <selection activeCell="A9" sqref="A9:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>